<commit_message>
1st commit for app.js
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8F841A-8A63-420B-B8D2-C088CDD9DBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99912A67-CE78-4209-A3A0-EFF564433050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>ziad</t>
+  </si>
+  <si>
+    <t>coco</t>
   </si>
 </sst>
 </file>
@@ -357,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -397,6 +400,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>